<commit_message>
Kien truc he thong
</commit_message>
<xml_diff>
--- a/Timepoints.xlsx
+++ b/Timepoints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BuiThanhDam02GmailGithub\DW_2023_T2_Nhom9\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\.Student\Nam4_HK1\Data Warehouse\DW_2023_T2_Nhom9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FEB168-B7D3-47C0-86FC-FEBD8290E7E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E1A215-8785-4C5F-BC19-1A2CF9DD645E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1008" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="51">
   <si>
     <t>Thành Viên</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>File load,trànform to warehouse (trello và drive)</t>
+  </si>
+  <si>
+    <t>29/10/2013</t>
   </si>
 </sst>
 </file>
@@ -492,7 +495,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -772,30 +775,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="10" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" style="53" customWidth="1"/>
-    <col min="6" max="6" width="36.44140625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="16" customWidth="1"/>
-    <col min="8" max="8" width="21.33203125" style="19" customWidth="1"/>
-    <col min="9" max="9" width="17.5546875" style="39" customWidth="1"/>
-    <col min="10" max="10" width="20.77734375" style="52" customWidth="1"/>
-    <col min="11" max="11" width="17.5546875" style="40" customWidth="1"/>
-    <col min="12" max="12" width="20.77734375" style="41" customWidth="1"/>
-    <col min="13" max="13" width="20.77734375" style="46" customWidth="1"/>
-    <col min="14" max="14" width="20.77734375" style="47" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="10"/>
+    <col min="1" max="1" width="15.140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" style="53" customWidth="1"/>
+    <col min="6" max="6" width="36.42578125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" style="16" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" style="19" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" style="39" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="52" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" style="40" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" style="41" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" style="46" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" style="47" customWidth="1"/>
+    <col min="15" max="16384" width="8.85546875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -838,7 +841,7 @@
       </c>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -863,7 +866,7 @@
       <c r="M2" s="42"/>
       <c r="N2" s="43"/>
     </row>
-    <row r="3" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -894,7 +897,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F4" s="26" t="s">
         <v>21</v>
       </c>
@@ -908,12 +911,20 @@
       <c r="J4" s="48">
         <v>44937</v>
       </c>
-      <c r="K4" s="37"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="44"/>
-      <c r="N4" s="45"/>
-    </row>
-    <row r="5" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K4" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="45" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F5" s="30" t="s">
         <v>22</v>
       </c>
@@ -932,7 +943,7 @@
       <c r="M5" s="44"/>
       <c r="N5" s="45"/>
     </row>
-    <row r="6" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F6" s="26" t="s">
         <v>23</v>
       </c>
@@ -949,7 +960,7 @@
       <c r="M6" s="44"/>
       <c r="N6" s="45"/>
     </row>
-    <row r="7" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F7" s="23" t="s">
         <v>24</v>
       </c>
@@ -964,7 +975,7 @@
       <c r="M7" s="42"/>
       <c r="N7" s="43"/>
     </row>
-    <row r="8" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F8" s="26" t="s">
         <v>25</v>
       </c>
@@ -983,7 +994,7 @@
       <c r="M8" s="44"/>
       <c r="N8" s="45"/>
     </row>
-    <row r="9" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="14"/>
       <c r="F9" s="26" t="s">
         <v>26</v>
@@ -1003,7 +1014,7 @@
       <c r="M9" s="44"/>
       <c r="N9" s="45"/>
     </row>
-    <row r="10" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="14"/>
       <c r="F10" s="26" t="s">
         <v>27</v>
@@ -1023,7 +1034,7 @@
       <c r="M10" s="44"/>
       <c r="N10" s="45"/>
     </row>
-    <row r="11" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="14"/>
       <c r="F11" s="23" t="s">
         <v>28</v>
@@ -1039,7 +1050,7 @@
       <c r="M11" s="42"/>
       <c r="N11" s="43"/>
     </row>
-    <row r="12" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="14"/>
       <c r="F12" s="26" t="s">
         <v>29</v>
@@ -1067,7 +1078,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="14"/>
       <c r="F13" s="26" t="s">
         <v>30</v>
@@ -1095,7 +1106,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="14"/>
       <c r="F14" s="26" t="s">
         <v>37</v>
@@ -1117,7 +1128,7 @@
       <c r="M14" s="44"/>
       <c r="N14" s="45"/>
     </row>
-    <row r="15" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="14"/>
       <c r="F15" s="26" t="s">
         <v>38</v>
@@ -1139,7 +1150,7 @@
       <c r="M15" s="44"/>
       <c r="N15" s="45"/>
     </row>
-    <row r="16" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="14"/>
       <c r="F16" s="26" t="s">
         <v>39</v>
@@ -1161,7 +1172,7 @@
       <c r="M16" s="44"/>
       <c r="N16" s="45"/>
     </row>
-    <row r="17" spans="3:14" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="14"/>
       <c r="F17" s="23" t="s">
         <v>31</v>
@@ -1177,7 +1188,7 @@
       <c r="M17" s="42"/>
       <c r="N17" s="43"/>
     </row>
-    <row r="18" spans="3:14" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="14"/>
       <c r="F18" s="26" t="s">
         <v>32</v>
@@ -1205,7 +1216,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="3:14" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="14"/>
       <c r="F19" s="26" t="s">
         <v>33</v>
@@ -1233,7 +1244,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="3:14" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="14"/>
       <c r="F20" s="26" t="s">
         <v>34</v>
@@ -1261,7 +1272,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="3:14" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="14"/>
       <c r="F21" s="26" t="s">
         <v>35</v>
@@ -1279,11 +1290,11 @@
       <c r="M21" s="44"/>
       <c r="N21" s="45"/>
     </row>
-    <row r="22" spans="3:14" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="14"/>
       <c r="J22" s="51"/>
     </row>
-    <row r="23" spans="3:14" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="14"/>
     </row>
   </sheetData>

</xml_diff>